<commit_message>
Code cleanup for submission.
</commit_message>
<xml_diff>
--- a/Data/Swarm_Dependencies.xlsx
+++ b/Data/Swarm_Dependencies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Umair Jamil\git\SWARM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88615A65-7ED6-4EFB-BEC4-14832041CF23}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28035485-AF3E-440A-8F70-7936AD753E4E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHP Pages" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
   <si>
     <t>Page</t>
   </si>
@@ -696,12 +696,15 @@
   <si>
     <t>DB link extension</t>
   </si>
+  <si>
+    <t>Status</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -734,16 +737,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -764,19 +786,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -814,59 +823,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -880,7 +842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -889,35 +851,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1034,21 +988,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1057,8 +996,12 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -1073,7 +1016,9 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -1114,7 +1059,9 @@
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -1131,39 +1078,6 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1186,6 +1100,73 @@
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1200,25 +1181,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:C22" totalsRowShown="0" headerRowDxfId="5" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Page" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Dependency" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:D22" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Page" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Dependency" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{EA6D566F-3A66-45F8-B56C-6FE96F821E81}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:E12" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:E12" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:E12" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="View" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Dependent" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Used Directly" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Comments" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="View" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Dependent" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Used Directly" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Comments" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1487,12 +1469,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,7 +1484,7 @@
     <col min="3" max="3" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1510,236 +1492,259 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="D22" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1754,7 +1759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>

</xml_diff>